<commit_message>
Adding the 300 character abstract for ICAT Day to source control.
</commit_message>
<xml_diff>
--- a/Documents/Data/DifferencesWithAudiveris.xlsx
+++ b/Documents/Data/DifferencesWithAudiveris.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="20380" windowHeight="16900" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8780" yWindow="4260" windowWidth="20380" windowHeight="11380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,8 +98,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -120,7 +130,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -129,6 +139,11 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -137,6 +152,11 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,7 +489,7 @@
   <dimension ref="B1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:N3"/>
+      <selection activeCell="G3" sqref="G3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -556,7 +576,7 @@
   <dimension ref="B1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="G3" sqref="G3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Backing up paper changes from overleaf. First full draft from start to finish!!!!!!!!
</commit_message>
<xml_diff>
--- a/Documents/Data/DifferencesWithAudiveris.xlsx
+++ b/Documents/Data/DifferencesWithAudiveris.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="4260" windowWidth="20380" windowHeight="11380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="14940" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="DifferenceAudiverisVsOriginal" sheetId="3" r:id="rId2"/>
+    <sheet name="PercentageAudiverisVsOrigin" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
     <t>Title</t>
   </si>
@@ -50,6 +52,27 @@
   </si>
   <si>
     <t>Divided By</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Dancing Clarinet</t>
+  </si>
+  <si>
+    <t>Mi Razon De Ser</t>
+  </si>
+  <si>
+    <t>Rudy</t>
+  </si>
+  <si>
+    <t>The Hobbit ...</t>
+  </si>
+  <si>
+    <t>The Rose</t>
+  </si>
+  <si>
+    <t>Complexity</t>
   </si>
 </sst>
 </file>
@@ -98,7 +121,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -126,11 +149,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -144,6 +189,16 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -157,11 +212,803 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Words</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$7:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Dancing Clarinet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mi Razon De Ser</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rudy</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Hobbit ...</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>The Rose</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$7:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>750.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1089.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8358.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9895.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>965.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4211.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Lines</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$7:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Dancing Clarinet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mi Razon De Ser</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rudy</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Hobbit ...</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>The Rose</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$7:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3386.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4699.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32940.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37449.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4392.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16573.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Characters</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$7:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Dancing Clarinet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mi Razon De Ser</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rudy</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Hobbit ...</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>The Rose</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$7:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>57876.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82813.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>608327.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>713595.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77706.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>308063.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Complexity</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$7:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Dancing Clarinet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mi Razon De Ser</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rudy</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Hobbit ...</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>The Rose</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$7:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>752.1770535714003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>168.6742754918996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159718.4751766055</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49994.10969672998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9530.843636363617</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>44032.85596775248</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2114946168"/>
+        <c:axId val="2114884664"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2114946168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2114884664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2114884664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2114946168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2800"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Words</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$7:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Dancing Clarinet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mi Razon De Ser</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rudy</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Hobbit ...</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>The Rose</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$G$7:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.256147540983607</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.276536312849162</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.436061981530756</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.471999618393436</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.218920145190563</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.331933119789505</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Lines</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$7:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Dancing Clarinet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mi Razon De Ser</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rudy</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Hobbit ...</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>The Rose</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$H$7:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.875840662183135</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.924454062561479</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.293743372216331</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.364361702127659</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.769716088328076</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>1.045623177483336</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Characters</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$7:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Dancing Clarinet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mi Razon De Ser</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rudy</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Hobbit ...</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>The Rose</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$I$7:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.679335641763014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.762368125494817</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.150728749917241</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.229136738975414</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.644226863097853</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.893159223849668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Complexity</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$7:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Dancing Clarinet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mi Razon De Ser</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rudy</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>The Hobbit ...</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>The Rose</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$J$7:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0667638386114615</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0131699772603012</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.632135163278108</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.252526678786299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.00323940227803</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.39356701204284</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2130667768"/>
+        <c:axId val="2132753992"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2130667768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2132753992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2132753992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2130667768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2800"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8561552" cy="5824483"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8561552" cy="5824483"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -486,10 +1333,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J3"/>
+  <dimension ref="B1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:J3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -558,6 +1405,151 @@
       </c>
       <c r="J3">
         <v>298655</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>2928</v>
+      </c>
+      <c r="D7">
+        <v>3866</v>
+      </c>
+      <c r="E7">
+        <v>85195</v>
+      </c>
+      <c r="F7">
+        <v>11266.234375</v>
+      </c>
+      <c r="G7">
+        <v>2838</v>
+      </c>
+      <c r="H7">
+        <v>3889</v>
+      </c>
+      <c r="I7">
+        <v>105455</v>
+      </c>
+      <c r="J7">
+        <v>12018.4114285714</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>3938</v>
+      </c>
+      <c r="D8">
+        <v>5083</v>
+      </c>
+      <c r="E8">
+        <v>108626</v>
+      </c>
+      <c r="F8">
+        <v>12807.4841860465</v>
+      </c>
+      <c r="G8">
+        <v>3852</v>
+      </c>
+      <c r="H8">
+        <v>5141</v>
+      </c>
+      <c r="I8">
+        <v>132065</v>
+      </c>
+      <c r="J8">
+        <v>12976.1584615384</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>19167</v>
+      </c>
+      <c r="D9">
+        <v>25461</v>
+      </c>
+      <c r="E9">
+        <v>528645</v>
+      </c>
+      <c r="F9">
+        <v>252665.06983782101</v>
+      </c>
+      <c r="G9">
+        <v>18575</v>
+      </c>
+      <c r="H9">
+        <v>27095</v>
+      </c>
+      <c r="I9">
+        <v>677243</v>
+      </c>
+      <c r="J9">
+        <v>92946.594661215495</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>20964</v>
+      </c>
+      <c r="D10">
+        <v>27448</v>
+      </c>
+      <c r="E10">
+        <v>580566</v>
+      </c>
+      <c r="F10">
+        <v>197975.55623434801</v>
+      </c>
+      <c r="G10">
+        <v>21457</v>
+      </c>
+      <c r="H10">
+        <v>30951</v>
+      </c>
+      <c r="I10">
+        <v>782696</v>
+      </c>
+      <c r="J10">
+        <v>247969.66593107799</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>4408</v>
+      </c>
+      <c r="D11">
+        <v>5706</v>
+      </c>
+      <c r="E11">
+        <v>120619</v>
+      </c>
+      <c r="F11">
+        <v>9500.0690909090808</v>
+      </c>
+      <c r="G11">
+        <v>4374</v>
+      </c>
+      <c r="H11">
+        <v>5713</v>
+      </c>
+      <c r="I11">
+        <v>151721</v>
+      </c>
+      <c r="J11">
+        <v>19030.912727272698</v>
       </c>
     </row>
   </sheetData>
@@ -573,10 +1565,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N3"/>
+  <dimension ref="B1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:J3"/>
+      <selection activeCell="G12" sqref="G12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -688,6 +1680,312 @@
       <c r="N3">
         <f>F3/Sheet1!J3</f>
         <v>0.27827761129061962</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
+      <c r="B7" t="str">
+        <f>Sheet1!B7</f>
+        <v>Dancing Clarinet</v>
+      </c>
+      <c r="C7">
+        <v>750</v>
+      </c>
+      <c r="D7">
+        <v>3386</v>
+      </c>
+      <c r="E7">
+        <v>57876</v>
+      </c>
+      <c r="F7" s="1">
+        <f>ABS(Sheet1!J7-Sheet1!F7)</f>
+        <v>752.17705357140039</v>
+      </c>
+      <c r="G7" s="2">
+        <f>C7/Sheet1!C7</f>
+        <v>0.25614754098360654</v>
+      </c>
+      <c r="H7" s="2">
+        <f>D7/Sheet1!D7</f>
+        <v>0.87584066218313505</v>
+      </c>
+      <c r="I7" s="2">
+        <f>E7/Sheet1!E7</f>
+        <v>0.67933564176301431</v>
+      </c>
+      <c r="J7" s="2">
+        <f>F7/Sheet1!F7</f>
+        <v>6.6763838611461554E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <f>C7/Sheet1!G7</f>
+        <v>0.26427061310782241</v>
+      </c>
+      <c r="L7" s="2">
+        <f>D7/Sheet1!H7</f>
+        <v>0.87066083826176399</v>
+      </c>
+      <c r="M7" s="2">
+        <f>E7/Sheet1!I7</f>
+        <v>0.54882177231994689</v>
+      </c>
+      <c r="N7" s="2">
+        <f>F7/Sheet1!J7</f>
+        <v>6.258539725002657E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
+      <c r="B8" t="str">
+        <f>Sheet1!B8</f>
+        <v>Mi Razon De Ser</v>
+      </c>
+      <c r="C8">
+        <v>1089</v>
+      </c>
+      <c r="D8">
+        <v>4699</v>
+      </c>
+      <c r="E8">
+        <v>82813</v>
+      </c>
+      <c r="F8" s="1">
+        <f>ABS(Sheet1!J8-Sheet1!F8)</f>
+        <v>168.67427549189961</v>
+      </c>
+      <c r="G8" s="2">
+        <f>C8/Sheet1!C8</f>
+        <v>0.27653631284916202</v>
+      </c>
+      <c r="H8" s="2">
+        <f>D8/Sheet1!D8</f>
+        <v>0.92445406256147944</v>
+      </c>
+      <c r="I8" s="2">
+        <f>E8/Sheet1!E8</f>
+        <v>0.76236812549481703</v>
+      </c>
+      <c r="J8" s="2">
+        <f>F8/Sheet1!F8</f>
+        <v>1.3169977260301198E-2</v>
+      </c>
+      <c r="K8" s="2">
+        <f>C8/Sheet1!G8</f>
+        <v>0.28271028037383178</v>
+      </c>
+      <c r="L8" s="2">
+        <f>D8/Sheet1!H8</f>
+        <v>0.91402450885041819</v>
+      </c>
+      <c r="M8" s="2">
+        <f>E8/Sheet1!I8</f>
+        <v>0.62706243137848783</v>
+      </c>
+      <c r="N8" s="2">
+        <f>F8/Sheet1!J8</f>
+        <v>1.2998783576191183E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="B9" t="str">
+        <f>Sheet1!B9</f>
+        <v>Rudy</v>
+      </c>
+      <c r="C9">
+        <v>8358</v>
+      </c>
+      <c r="D9">
+        <v>32940</v>
+      </c>
+      <c r="E9">
+        <v>608327</v>
+      </c>
+      <c r="F9" s="1">
+        <f>ABS(Sheet1!J9-Sheet1!F9)</f>
+        <v>159718.47517660551</v>
+      </c>
+      <c r="G9" s="2">
+        <f>C9/Sheet1!C9</f>
+        <v>0.43606198153075598</v>
+      </c>
+      <c r="H9" s="2">
+        <f>D9/Sheet1!D9</f>
+        <v>1.293743372216331</v>
+      </c>
+      <c r="I9" s="2">
+        <f>E9/Sheet1!E9</f>
+        <v>1.1507287499172412</v>
+      </c>
+      <c r="J9" s="2">
+        <f>F9/Sheet1!F9</f>
+        <v>0.63213516327810793</v>
+      </c>
+      <c r="K9" s="2">
+        <f>C9/Sheet1!G9</f>
+        <v>0.44995962314939436</v>
+      </c>
+      <c r="L9" s="2">
+        <f>D9/Sheet1!H9</f>
+        <v>1.2157224580180845</v>
+      </c>
+      <c r="M9" s="2">
+        <f>E9/Sheet1!I9</f>
+        <v>0.89824036571806576</v>
+      </c>
+      <c r="N9" s="2">
+        <f>F9/Sheet1!J9</f>
+        <v>1.7183897458402788</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14">
+      <c r="B10" t="str">
+        <f>Sheet1!B10</f>
+        <v>The Hobbit ...</v>
+      </c>
+      <c r="C10">
+        <v>9895</v>
+      </c>
+      <c r="D10">
+        <v>37449</v>
+      </c>
+      <c r="E10">
+        <v>713595</v>
+      </c>
+      <c r="F10" s="1">
+        <f>ABS(Sheet1!J10-Sheet1!F10)</f>
+        <v>49994.109696729982</v>
+      </c>
+      <c r="G10" s="2">
+        <f>C10/Sheet1!C10</f>
+        <v>0.47199961839343635</v>
+      </c>
+      <c r="H10" s="2">
+        <f>D10/Sheet1!D10</f>
+        <v>1.3643617021276595</v>
+      </c>
+      <c r="I10" s="2">
+        <f>E10/Sheet1!E10</f>
+        <v>1.2291367389754138</v>
+      </c>
+      <c r="J10" s="2">
+        <f>F10/Sheet1!F10</f>
+        <v>0.25252667878629853</v>
+      </c>
+      <c r="K10" s="2">
+        <f>C10/Sheet1!G10</f>
+        <v>0.46115486787528548</v>
+      </c>
+      <c r="L10" s="2">
+        <f>D10/Sheet1!H10</f>
+        <v>1.2099447513812154</v>
+      </c>
+      <c r="M10" s="2">
+        <f>E10/Sheet1!I10</f>
+        <v>0.91171412655743733</v>
+      </c>
+      <c r="N10" s="2">
+        <f>F10/Sheet1!J10</f>
+        <v>0.20161381235487735</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14">
+      <c r="B11" t="str">
+        <f>Sheet1!B11</f>
+        <v>The Rose</v>
+      </c>
+      <c r="C11">
+        <v>965</v>
+      </c>
+      <c r="D11">
+        <v>4392</v>
+      </c>
+      <c r="E11">
+        <v>77706</v>
+      </c>
+      <c r="F11" s="1">
+        <f>ABS(Sheet1!J11-Sheet1!F11)</f>
+        <v>9530.8436363636174</v>
+      </c>
+      <c r="G11" s="2">
+        <f>C11/Sheet1!C11</f>
+        <v>0.2189201451905626</v>
+      </c>
+      <c r="H11" s="2">
+        <f>D11/Sheet1!D11</f>
+        <v>0.7697160883280757</v>
+      </c>
+      <c r="I11" s="2">
+        <f>E11/Sheet1!E11</f>
+        <v>0.6442268630978536</v>
+      </c>
+      <c r="J11" s="2">
+        <f>F11/Sheet1!F11</f>
+        <v>1.0032394022780304</v>
+      </c>
+      <c r="K11" s="2">
+        <f>C11/Sheet1!G11</f>
+        <v>0.22062185642432555</v>
+      </c>
+      <c r="L11" s="2">
+        <f>D11/Sheet1!H11</f>
+        <v>0.7687729739191318</v>
+      </c>
+      <c r="M11" s="2">
+        <f>E11/Sheet1!I11</f>
+        <v>0.51216377429624116</v>
+      </c>
+      <c r="N11" s="2">
+        <f>F11/Sheet1!J11</f>
+        <v>0.50080854097476979</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f>AVERAGE(C7:C11)</f>
+        <v>4211.3999999999996</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:E12" si="0">AVERAGE(D7:D11)</f>
+        <v>16573.2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>308063.40000000002</v>
+      </c>
+      <c r="F12">
+        <f>AVERAGE(F7:F11)</f>
+        <v>44032.855967752483</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:I12" si="1">AVERAGE(G7:G11)</f>
+        <v>0.33193311978950468</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>1.045623177483336</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0.89315922384966806</v>
+      </c>
+      <c r="J12">
+        <f>AVERAGE(J7:J11)</f>
+        <v>0.39356701204283995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>